<commit_message>
Hide the maze door, Add goal trigger, Update Documents
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0880FF91-669B-40CF-89D7-6296A6C30AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFC4545-1C79-4987-BF86-60B63E7DDE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
   <sheets>
-    <sheet name="やる事＆気づいた事" sheetId="1" r:id="rId1"/>
-    <sheet name="出来ている事" sheetId="2" r:id="rId2"/>
+    <sheet name="やる事" sheetId="1" r:id="rId1"/>
+    <sheet name="気づいた不具合" sheetId="3" r:id="rId2"/>
+    <sheet name="思い付いた事" sheetId="4" r:id="rId3"/>
+    <sheet name="出来ている事" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -78,13 +80,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>スタートエリアとダンジョンエリアの基礎</t>
-    <rPh sb="17" eb="19">
-      <t>キソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ダンジョンエリアでESCキーを押したらスタートエリアに戻れる</t>
     <rPh sb="15" eb="16">
       <t>オ</t>
@@ -142,26 +137,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>メニュー画面など（オプションでカメラ感度を調整できるの欲しい）</t>
-    <rPh sb="4" eb="6">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>カンド</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>チョウセイ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ホ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スキルアイコン？</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>スタートエリアとダンジョンエリアの装飾</t>
     <rPh sb="17" eb="19">
       <t>ソウショク</t>
@@ -183,26 +158,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>敵をリスポーンする仕組み</t>
-    <rPh sb="0" eb="1">
-      <t>テキ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>シク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>スキル＆アニメーション＆当たり判定</t>
-    <rPh sb="12" eb="13">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ハンテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>状況</t>
     <rPh sb="0" eb="2">
       <t>ジョウキョウ</t>
@@ -210,17 +165,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ボスキャラ＆ボスエリア</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>チョン予定</t>
-    <rPh sb="3" eb="5">
-      <t>ヨテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>HP表示？（個人的にはHP表示しないのが面白いと思う派）</t>
     <rPh sb="2" eb="4">
       <t>ヒョウジ</t>
@@ -251,35 +195,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ワープ装置、木や石のモデルなどインポート済み</t>
-    <rPh sb="3" eb="5">
-      <t>ソウチ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>イシ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ズ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>インベントリ的なやつ（ダンジョンで拾ったコインを覚えておくやつとか）</t>
-    <rPh sb="6" eb="7">
-      <t>テキ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ヒロ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>オボ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ランダムに動く敵たち（プレイヤーが視野に入ったら近づくぐらいのAIをとりあえず目標にする）　→　まずはコインをランダムに置く</t>
     <rPh sb="5" eb="6">
       <t>ウゴ</t>
@@ -361,6 +276,348 @@
     </rPh>
     <rPh sb="34" eb="35">
       <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>機能</t>
+    <rPh sb="0" eb="2">
+      <t>キノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>セーブシステム（今は保存する対象はダンジョン内で集めたコインの数のみ）</t>
+    <rPh sb="8" eb="9">
+      <t>イマ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>アツ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダンジョン内にランダムにコインを生成＆それを拾える＆スタートエリアに戻っても数を覚えておく仕組み</t>
+    <rPh sb="5" eb="6">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ヒロ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>オボ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>シク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>対応済み</t>
+    <rPh sb="0" eb="3">
+      <t>タイオウズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>対応済み</t>
+    <rPh sb="0" eb="3">
+      <t>タイオウズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>不具合</t>
+    <rPh sb="0" eb="3">
+      <t>フグアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>たまに、ダンジョンをすり抜けてプレイヤーが下に落ちてしまう、、、</t>
+    <rPh sb="12" eb="13">
+      <t>ヌ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>オ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ステージにBGMを入れる</t>
+    <rPh sb="9" eb="10">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アクション（スキル＆アニメーション＆当たり判定）</t>
+    <rPh sb="18" eb="19">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ハンテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダンジョンで拾ったコインを他のシーンでも見れる様に覚えておく仕組み（セーブする対象を保持する器的なもの）</t>
+    <rPh sb="6" eb="7">
+      <t>ヒロ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>オボ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>シク</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ホジ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ウツワテキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スタートエリアとダンジョンエリアのベース</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開発用</t>
+    <rPh sb="0" eb="3">
+      <t>カイハツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダンジョンエリアのゴール（白い箱）に触れるとスタートエリアに戻る</t>
+    <rPh sb="13" eb="14">
+      <t>シロ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ハコ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>敵へのロックオン</t>
+    <rPh sb="0" eb="1">
+      <t>テキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チョン作業予定</t>
+    <rPh sb="3" eb="7">
+      <t>サギョウヨテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ワープ装置、木や石などの3Dモデルをインポート</t>
+    <rPh sb="3" eb="5">
+      <t>ソウチ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>イシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チョン調査中</t>
+    <rPh sb="3" eb="5">
+      <t>チョウサ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チョン作業予定</t>
+    <rPh sb="3" eb="7">
+      <t>サギョウヨテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボス戦（ボスキャラ＆ボスエリア＆ギミック）</t>
+    <rPh sb="2" eb="3">
+      <t>セン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スキルアイコン表示？（ソシャゲっぽくなりすぎか）</t>
+    <rPh sb="7" eb="9">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダンジョンの２Dマップ（必要か要検討）→　コインを払ってマップ解放とか</t>
+    <rPh sb="12" eb="14">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t>ヨウケントウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ハラ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カイホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジャンプアクション（スキルにして踏んで敵を倒せるようにするか）→　スペースキーを想定</t>
+    <rPh sb="16" eb="17">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>タオ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ソウテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニュー画面など（オプションでカメラ感度を調整できるの欲しい）→　ESCキーで出す＆ダンジョン脱出キーを他のに変える</t>
+    <rPh sb="4" eb="6">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>カンド</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>チョウセイ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ホ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ダッシュツ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>敵をリスポーンする仕組み&amp;プレイヤーを見つけたら近づいてくる敵</t>
+    <rPh sb="0" eb="1">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>シク</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>テキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダッシュアクション（ワリオの体当たりみたいなスキル）→　これで敵を攻撃出来るイメージ　→　他のキーとのコンビネーションなしの通常マウス左クリックとか</t>
+    <rPh sb="67" eb="68">
+      <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スキルストア（コインを払ってスキルを取得するとかステータスを上げるとか出来る所）→　商人でもよい</t>
+    <rPh sb="11" eb="12">
+      <t>ハラ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シュトク</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>デキ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>トコロ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ショウニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アイテムウィンドウ（必要？）→イメージとしてはIキーを押したら出てくる</t>
+    <rPh sb="10" eb="12">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>デ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -386,12 +643,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -408,8 +671,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -726,18 +995,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF443F6F-3FD6-43F7-BBB2-838A80979D3C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="127.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
@@ -748,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -756,13 +1025,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -770,57 +1039,69 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -828,10 +1109,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -839,12 +1120,9 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -853,13 +1131,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -867,13 +1145,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -881,79 +1156,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -964,18 +1173,247 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59605722-557F-4DE1-86F0-1F7C562827BD}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2A5B18-39DE-4831-9996-C9E954F67B66}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CBB20-83FA-434C-BC5A-137CF52FA55C}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="154.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59605722-557F-4DE1-86F0-1F7C562827BD}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
@@ -991,7 +1429,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1002,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1013,7 +1451,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1024,10 +1462,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1035,10 +1473,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1046,10 +1484,43 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add jump action and fall action
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFC4545-1C79-4987-BF86-60B63E7DDE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0457E8-25C2-4E48-9B71-CE915FC1CB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -37,16 +37,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>とりあえずWASDでの前後左右移動</t>
-    <rPh sb="11" eb="15">
-      <t>ゼンゴサユウ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>分類</t>
     <rPh sb="0" eb="2">
       <t>ブンルイ</t>
@@ -54,25 +44,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>マウス移動でキャラクターの周りを衛星の様に回る</t>
-    <rPh sb="3" eb="5">
-      <t>イドウ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>マワ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>エイセイ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>マワ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>BGMをいくつかダウンロード済み</t>
     <rPh sb="14" eb="15">
       <t>ズ</t>
@@ -487,13 +458,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ボス戦（ボスキャラ＆ボスエリア＆ギミック）</t>
-    <rPh sb="2" eb="3">
-      <t>セン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>スキルアイコン表示？（ソシャゲっぽくなりすぎか）</t>
     <rPh sb="7" eb="9">
       <t>ヒョウジ</t>
@@ -580,13 +544,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ダッシュアクション（ワリオの体当たりみたいなスキル）→　これで敵を攻撃出来るイメージ　→　他のキーとのコンビネーションなしの通常マウス左クリックとか</t>
-    <rPh sb="67" eb="68">
-      <t>ヒダリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>スキルストア（コインを払ってスキルを取得するとかステータスを上げるとか出来る所）→　商人でもよい</t>
     <rPh sb="11" eb="12">
       <t>ハラ</t>
@@ -618,6 +575,77 @@
     </rPh>
     <rPh sb="31" eb="32">
       <t>デ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダッシュアクション（ワリオの体当たりみたいなスキル）→　これで敵を攻撃出来るイメージ　→　他のキーとのコンビネーションなしの通常マウス右クリックとか</t>
+    <rPh sb="67" eb="68">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>マウス移動でカメラがキャラクターの周りを衛星の様に回る</t>
+    <rPh sb="3" eb="5">
+      <t>イドウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>エイセイ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>マワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>保留</t>
+    <rPh sb="0" eb="2">
+      <t>ホリュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>とりあえずWASDでの前後左右移動＆Shift押したら走る</t>
+    <rPh sb="11" eb="15">
+      <t>ゼンゴサユウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>イドウ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ハシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボス戦（ボスキャラ＆ボスエリア＆ギミック）→　ボスは主人公のライバルでエンディングにも出てきて「まだ追ってくるのかこいつ」的な流れ</t>
+    <rPh sb="2" eb="3">
+      <t>セン</t>
+    </rPh>
+    <rPh sb="26" eb="29">
+      <t>シュジンコウ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ナガ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -671,14 +699,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -998,7 +1023,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1011,13 +1036,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -1025,13 +1050,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -1039,13 +1064,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1053,27 +1078,27 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>48</v>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1081,13 +1106,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1095,13 +1120,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -1109,10 +1134,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
+      <c r="D8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -1120,10 +1148,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -1131,13 +1162,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -1145,10 +1176,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -1156,13 +1187,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1177,7 +1208,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1190,13 +1221,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -1204,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -1218,13 +1249,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1232,13 +1263,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -1246,13 +1277,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1266,7 +1297,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1279,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1290,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1301,10 +1332,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1312,10 +1343,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1323,10 +1354,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1334,10 +1365,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1345,10 +1376,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -1356,10 +1387,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -1367,10 +1398,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -1378,10 +1409,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
@@ -1389,15 +1420,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1406,7 +1438,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1418,7 +1450,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1429,10 +1461,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1440,10 +1472,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1451,10 +1483,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1462,10 +1494,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1473,10 +1505,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1484,10 +1516,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -1495,10 +1527,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -1506,10 +1538,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -1517,10 +1549,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File Organization, some tweak, update task document
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36514ACC-51BE-4F3A-A47A-8B929ED9DF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014C76E4-0F6E-4D33-B6F9-5F01880E1592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
@@ -1148,7 +1148,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1419,7 +1419,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1497,18 +1497,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D6" t="s">
-        <v>39</v>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1652,7 +1652,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Add test skill to key 1 and player combat to key 2
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48F37CB-BFE3-4EF1-A99A-98C2830101F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D0558B-8E37-43FA-A54A-3382208F2A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
   <sheets>
     <sheet name="やる事" sheetId="1" r:id="rId1"/>
@@ -441,16 +441,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>チョン調査中</t>
-    <rPh sb="3" eb="5">
-      <t>チョウサ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>チュウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>スキルアイコン表示？（ソシャゲっぽくなりすぎか）</t>
     <rPh sb="7" eb="9">
       <t>ヒョウジ</t>
@@ -788,6 +778,13 @@
     </rPh>
     <rPh sb="28" eb="29">
       <t>プン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>対応済み...?</t>
+    <rPh sb="0" eb="3">
+      <t>タイオウズ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1168,7 +1165,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1198,7 +1195,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>26</v>
@@ -1237,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
@@ -1298,7 +1295,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1326,7 +1323,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>26</v>
@@ -1337,10 +1334,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
@@ -1351,10 +1348,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>26</v>
@@ -1365,10 +1362,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
@@ -1379,10 +1376,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1390,10 +1387,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>26</v>
@@ -1404,10 +1401,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
@@ -1418,10 +1415,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
         <v>37</v>
@@ -1439,7 +1436,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1503,18 +1500,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1522,10 +1519,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>26</v>
@@ -1541,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CBB20-83FA-434C-BC5A-137CF52FA55C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1569,7 +1566,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1591,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1602,7 +1599,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1646,7 +1643,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -1657,7 +1654,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
@@ -1665,10 +1662,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
         <v>67</v>
-      </c>
-      <c r="C11" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1682,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59605722-557F-4DE1-86F0-1F7C562827BD}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1709,7 +1706,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1720,7 +1717,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1805,10 +1802,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -1816,10 +1813,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
@@ -1830,7 +1827,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Add Spider Web Attack
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369E7D3E-1908-4E87-BDDC-F96186110058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420103E4-143C-42AC-BBD3-397C14B0FD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-240" windowWidth="18240" windowHeight="28440" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
   <sheets>
     <sheet name="やる事" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -900,6 +900,64 @@
     </rPh>
     <rPh sb="14" eb="17">
       <t>コウゲキリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>システム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボールのバウンド（敵の攻撃用？）</t>
+    <rPh sb="9" eb="10">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時間内に取ったら報酬がでかい物（ダンジョン内のどっかにある）</t>
+    <rPh sb="0" eb="3">
+      <t>ジカンナイ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ホウシュウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>モノ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ナイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メタルスラッグのボス戦の様によけづらい玉が大量に出るボス戦</t>
+    <rPh sb="10" eb="11">
+      <t>セン</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>タマ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>タイリョウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>セン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1283,15 +1341,15 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="154.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1302,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1316,7 +1374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1327,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1341,7 +1399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1355,7 +1413,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1369,7 +1427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1383,7 +1441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1394,7 +1452,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1405,7 +1463,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1419,7 +1477,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1430,7 +1488,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1444,7 +1502,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1458,7 +1516,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1472,7 +1530,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1486,7 +1544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1497,7 +1555,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1511,7 +1569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1525,7 +1583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1539,7 +1597,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1553,7 +1611,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1582,15 +1640,15 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.35546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1601,7 +1659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1615,7 +1673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1629,7 +1687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1643,7 +1701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1657,7 +1715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1671,23 +1729,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="18" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="19" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="20" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="21" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="22" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="23" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="26" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="27" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="28" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="29" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="30" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="31" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="32" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.65"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1696,21 +1754,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CBB20-83FA-434C-BC5A-137CF52FA55C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="154.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.2109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.65">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1718,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1729,7 +1787,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1740,7 +1798,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1751,7 +1809,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1762,7 +1820,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1773,7 +1831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1784,7 +1842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1795,7 +1853,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1806,7 +1864,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1817,7 +1875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1828,7 +1886,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1837,6 +1895,39 @@
       </c>
       <c r="C12" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.65">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.65">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.65">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1851,17 +1942,17 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.65">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1869,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1880,7 +1971,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1891,7 +1982,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1902,7 +1993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1913,7 +2004,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1924,7 +2015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1935,7 +2026,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1946,7 +2037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1957,7 +2048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1968,7 +2059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1979,7 +2070,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1990,7 +2081,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2001,7 +2092,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2012,7 +2103,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2023,7 +2114,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.65">
       <c r="C21" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Aim And Throw State
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420103E4-143C-42AC-BBD3-397C14B0FD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A87E34-705F-4DD5-B2A0-8F92C1402BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
+    <workbookView xWindow="-18120" yWindow="-240" windowWidth="18240" windowHeight="28440" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
   <sheets>
     <sheet name="やる事" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -958,6 +958,47 @@
     </rPh>
     <rPh sb="28" eb="29">
       <t>セン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スキルはマリオカートのアイテム取得を真似する？</t>
+    <rPh sb="15" eb="17">
+      <t>シュトク</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>マネ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>敵は振り回すのではなく、ゴッドオブウォーの斧を投げるのを真似する？敵がぶつかったら爆発が起こる</t>
+    <rPh sb="0" eb="1">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>フ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>オノ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>マネ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>バクハツ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>オ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1341,15 +1382,15 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="154.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1374,7 +1415,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1385,7 +1426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1399,7 +1440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1413,7 +1454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1427,7 +1468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1441,7 +1482,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1452,7 +1493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1463,7 +1504,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1477,7 +1518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1488,7 +1529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1502,7 +1543,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1516,7 +1557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1530,7 +1571,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1544,7 +1585,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1555,7 +1596,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1569,7 +1610,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1583,7 +1624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1597,7 +1638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1611,7 +1652,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1640,15 +1681,15 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.35546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1659,7 +1700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1673,7 +1714,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1687,7 +1728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1701,7 +1742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1715,7 +1756,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1729,23 +1770,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="18" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="19" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="20" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="21" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="22" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="23" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="26" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="27" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="28" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="29" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="30" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="31" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="32" customFormat="1" x14ac:dyDescent="0.65"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.65"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1754,21 +1795,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CBB20-83FA-434C-BC5A-137CF52FA55C}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="154.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.2109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1776,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1787,7 +1828,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1798,7 +1839,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1809,7 +1850,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1820,7 +1861,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1831,7 +1872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1842,7 +1883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1853,7 +1894,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1864,7 +1905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1875,7 +1916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1886,7 +1927,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1897,7 +1938,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1908,7 +1949,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1919,7 +1960,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1928,6 +1969,28 @@
       </c>
       <c r="C15" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1945,14 +2008,14 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1960,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1971,7 +2034,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1982,7 +2045,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1993,7 +2056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2004,7 +2067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2015,7 +2078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2026,7 +2089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2037,7 +2100,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2048,7 +2111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2059,7 +2122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2070,7 +2133,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2081,7 +2144,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2092,7 +2155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2103,7 +2166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2114,7 +2177,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.65">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C21" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Document and NPC
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E83B1A-4B81-4315-BF89-038D4DCD3DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C45EA-BA78-4D91-9BC3-3852FC724829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-240" windowWidth="18240" windowHeight="28440" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
   <sheets>
     <sheet name="やる事" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -1045,6 +1045,55 @@
     </rPh>
     <rPh sb="44" eb="45">
       <t>シマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コンセプト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Wormsの様にコミカルな武器or攻撃</t>
+    <rPh sb="6" eb="7">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ブキ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウゲキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スピード、スタミナ、パワー、根性、賢さ</t>
+    <rPh sb="14" eb="16">
+      <t>コンジョウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カシコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>女の子を守る男の子（ICO、メイドインアビス、ワンダと巨像）</t>
+    <rPh sb="0" eb="1">
+      <t>オンナ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>マモ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>オトコ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>キョゾウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1841,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CBB20-83FA-434C-BC5A-137CF52FA55C}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2070,6 +2119,39 @@
       </c>
       <c r="C20" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some animations and objects for cutscene
</commit_message>
<xml_diff>
--- a/Indie Game Challenge/Assets/Document/タスク.xlsx
+++ b/Indie Game Challenge/Assets/Document/タスク.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JungWonchul\Indie_Game_Challenge\Indie Game Challenge\Assets\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C45EA-BA78-4D91-9BC3-3852FC724829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4FA97D-1E40-4129-98A8-B115F03530BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
+    <workbookView xWindow="-18120" yWindow="-240" windowWidth="18240" windowHeight="28440" activeTab="2" xr2:uid="{622E737B-4981-43F7-9D0E-EEB3C697A13C}"/>
   </bookViews>
   <sheets>
     <sheet name="やる事" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
   <si>
     <t>内容</t>
     <rPh sb="0" eb="2">
@@ -1094,6 +1094,129 @@
     </rPh>
     <rPh sb="27" eb="29">
       <t>キョゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BGM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コード進行：F5-E5-Bdim</t>
+    <rPh sb="3" eb="5">
+      <t>シンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自動に近い敵に球を定期的に一発ずつ撃つ＋距離が近くなったら物理攻撃に変わる</t>
+    <rPh sb="0" eb="2">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>タマ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>テイキテキ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>イッパツ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>キョリ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>チカ</t>
+    </rPh>
+    <rPh sb="29" eb="33">
+      <t>ブツリコウゲキ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キャラクター</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>波に飲み込まれている事実に気づかず、自分がその波に乗っていると錯覚している住民</t>
+    <rPh sb="0" eb="1">
+      <t>ナミ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ジジツ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ナミ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>サッカク</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ジュウミン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>眼が一つしかなく反対側の景色が見えていないのにも関わらず、見えている風景がすべてだと思い込んでいる住民</t>
+    <rPh sb="0" eb="1">
+      <t>メ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>ハンタイガワ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ケシキ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>カカ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>フウケイ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ジュウミン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1474,7 +1597,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1890,16 +2013,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CBB20-83FA-434C-BC5A-137CF52FA55C}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="154.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
   </cols>
@@ -2152,6 +2275,50 @@
       </c>
       <c r="C23" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>